<commit_message>
Updated templates as per CIS Added CIS Features Modified region_dict for OCI Regions
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-EN-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-EN-template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PycharmProjects\oci_develop\oci_tenancy\SetUpOCI_Via_TF\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SUSINGLA\Desktop\Misc\CD3aaS\CD3 Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22990" windowHeight="8280"/>
   </bookViews>
   <sheets>
     <sheet name="Release-Info" sheetId="1" r:id="rId1"/>
@@ -4099,7 +4099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -4530,8 +4530,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
DRGv2 Support and code optimization for export process
</commit_message>
<xml_diff>
--- a/oci_tenancy/SetUpOCI_Via_TF/example/CD3-EN-template.xlsx
+++ b/oci_tenancy/SetUpOCI_Via_TF/example/CD3-EN-template.xlsx
@@ -2126,7 +2126,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>v7.2</t>
+      <t xml:space="preserve">v8.0
+</t>
     </r>
     <r>
       <rPr>
@@ -2136,9 +2137,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">
-CD3 Sheet Format is same as release v7.0
-Added additional components to Groups, Policies, Tags as per CIS compliance
+      <t xml:space="preserve">Added new sheets - DRGv2 and DRGRouteRulesinOCI
 </t>
     </r>
   </si>
@@ -2182,6 +2181,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>

</xml_diff>